<commit_message>
Updated Questions Scheme and Scrum Report
</commit_message>
<xml_diff>
--- a/src/main/resources/סכמה לשאלות.csv.xlsx
+++ b/src/main/resources/סכמה לשאלות.csv.xlsx
@@ -3,24 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campushaifaac-my.sharepoint.com/personal/lhallumi_campus_haifa_ac_il/Documents/Desktop/software engineering/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D02AEF6-9D83-4FFB-B0BB-B877F604996E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D647F1F8-2E1E-424C-96D5-EB72E921C0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{D0ED07A3-AFA2-4C93-BE2D-3198A7060C86}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D0ED07A3-AFA2-4C93-BE2D-3198A7060C86}"/>
   </bookViews>
   <sheets>
     <sheet name="סכמה לשאלות" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -46,19 +42,334 @@
     <t>Correct Answer</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>apple</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>hat</t>
+    <t>What is the main purpose of system modeling?</t>
+  </si>
+  <si>
+    <t>Which UML diagram shows interactions between a system and its environment?</t>
+  </si>
+  <si>
+    <t>Which requirement type describes what the system must do?</t>
+  </si>
+  <si>
+    <t>What is verification concerned with?</t>
+  </si>
+  <si>
+    <t>A design pattern is best described as:</t>
+  </si>
+  <si>
+    <t>What is the main function of a review?</t>
+  </si>
+  <si>
+    <t>Which perspective models how components interact inside a system?</t>
+  </si>
+  <si>
+    <t>What is a major problem with natural-language requirements?</t>
+  </si>
+  <si>
+    <t>In the project life cycle, when does integration testing occur?</t>
+  </si>
+  <si>
+    <t>What does the Singleton pattern ensure?</t>
+  </si>
+  <si>
+    <t>Which model is most suitable for event-driven reactive systems?</t>
+  </si>
+  <si>
+    <t>Which type of review is usually conducted at major project milestones and focuses on approval?</t>
+  </si>
+  <si>
+    <t>Which requirement type often affects overall system architecture rather than individual components?</t>
+  </si>
+  <si>
+    <t>In UML sequence diagrams, what do lifelines represent?</t>
+  </si>
+  <si>
+    <t>Which activity in requirements engineering resolves conflicting requirements?</t>
+  </si>
+  <si>
+    <t>What is the main drawback of depending only on interviews for requirements elicitation?</t>
+  </si>
+  <si>
+    <t>Code inspection has what approximate defect removal effectiveness?</t>
+  </si>
+  <si>
+    <t>Which design activity involves identifying principal objects and their relationships?</t>
+  </si>
+  <si>
+    <t>Why are domain requirements often difficult for software engineers to understand?</t>
+  </si>
+  <si>
+    <t>What is a major consequence of poor system boundary definition in context modeling?</t>
+  </si>
+  <si>
+    <t>In the SQA defect removal cost model, why is solving a defect during operation extremely expensive?</t>
+  </si>
+  <si>
+    <t>What is a key reason UML is less useful for dynamically typed languages like Python?</t>
+  </si>
+  <si>
+    <t>During detailed design, what is the main focus?</t>
+  </si>
+  <si>
+    <t>What is one major indirect objective of conducting technical reviews?</t>
+  </si>
+  <si>
+    <t>To replace the final system implementation</t>
+  </si>
+  <si>
+    <t>Class diagram</t>
+  </si>
+  <si>
+    <t>Non-functional requirements</t>
+  </si>
+  <si>
+    <t>Ensuring the system meets user expectations</t>
+  </si>
+  <si>
+    <t>A UML notation</t>
+  </si>
+  <si>
+    <t>To rewrite project requirements</t>
+  </si>
+  <si>
+    <t>Interaction perspective</t>
+  </si>
+  <si>
+    <t>They require programming knowledge</t>
+  </si>
+  <si>
+    <t>Before implementation</t>
+  </si>
+  <si>
+    <t>That multiple instances can run in parallel</t>
+  </si>
+  <si>
+    <t>Use case diagram</t>
+  </si>
+  <si>
+    <t>Peer review</t>
+  </si>
+  <si>
+    <t>The time between events</t>
+  </si>
+  <si>
+    <t>Requirements validation</t>
+  </si>
+  <si>
+    <t>They take too long</t>
+  </si>
+  <si>
+    <t>Requirements engineering</t>
+  </si>
+  <si>
+    <t>They are expressed in application-specific language unfamiliar to engineers</t>
+  </si>
+  <si>
+    <t>Incorrect system behavior modeling</t>
+  </si>
+  <si>
+    <t>It requires rewriting documentation</t>
+  </si>
+  <si>
+    <t>Python does not support classes</t>
+  </si>
+  <si>
+    <t>Determining system boundaries</t>
+  </si>
+  <si>
+    <t>Delivering a final product</t>
+  </si>
+  <si>
+    <t>To develop abstract models showing different system perspectives</t>
+  </si>
+  <si>
+    <t>User experience requirements</t>
+  </si>
+  <si>
+    <t>Ensuring the system is bug-free</t>
+  </si>
+  <si>
+    <t>A reusable solution to a recurring design problem</t>
+  </si>
+  <si>
+    <t>To detect errors and evaluate a work product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structural perspective </t>
+  </si>
+  <si>
+    <t>They may be ambiguous and unclear</t>
+  </si>
+  <si>
+    <t>During contract review</t>
+  </si>
+  <si>
+    <t>That the system runs faster</t>
+  </si>
+  <si>
+    <t>State machine model</t>
+  </si>
+  <si>
+    <t>Walkthrough</t>
+  </si>
+  <si>
+    <t>User requirements</t>
+  </si>
+  <si>
+    <t>The decomposition of classes into attributes</t>
+  </si>
+  <si>
+    <t>Requirements prioritization and negotiation</t>
+  </si>
+  <si>
+    <t>They cannot capture domain-specific knowledge fully</t>
+  </si>
+  <si>
+    <t>Architectural design</t>
+  </si>
+  <si>
+    <t>They include too many UML diagrams</t>
+  </si>
+  <si>
+    <t>Increased political conflicts and misallocated workloads</t>
+  </si>
+  <si>
+    <t>It delays integration</t>
+  </si>
+  <si>
+    <t>UML is optimized for static typing and compile-time structures</t>
+  </si>
+  <si>
+    <t>Designing test cases</t>
+  </si>
+  <si>
+    <t>Training team members and transferring knowledge</t>
+  </si>
+  <si>
+    <t>To generate test cases automatically</t>
+  </si>
+  <si>
+    <t>State diagram</t>
+  </si>
+  <si>
+    <t>Domain requirements</t>
+  </si>
+  <si>
+    <t>Ensuring the product matches earlier-phase specifications</t>
+  </si>
+  <si>
+    <t>A coding convention</t>
+  </si>
+  <si>
+    <t>To execute the program</t>
+  </si>
+  <si>
+    <t>Behavioral perspective</t>
+  </si>
+  <si>
+    <t>They are too mathematical</t>
+  </si>
+  <si>
+    <t>Before requirements validation</t>
+  </si>
+  <si>
+    <t>That only one instance of a class exists</t>
+  </si>
+  <si>
+    <t>Activity diagram</t>
+  </si>
+  <si>
+    <t>Formal review</t>
+  </si>
+  <si>
+    <t>Functional requirements</t>
+  </si>
+  <si>
+    <t>The static structure of the system</t>
+  </si>
+  <si>
+    <t>Requirements discovery</t>
+  </si>
+  <si>
+    <t>They are too structured</t>
+  </si>
+  <si>
+    <t>Object-oriented detailed design</t>
+  </si>
+  <si>
+    <t>They contain excessive mathematical notation</t>
+  </si>
+  <si>
+    <t>Limited design flexibility</t>
+  </si>
+  <si>
+    <t>It must be solved by senior managers</t>
+  </si>
+  <si>
+    <t>Python lacks diagramming tools</t>
+  </si>
+  <si>
+    <t>Specifying module-level data structures and algorithms</t>
+  </si>
+  <si>
+    <t>Reducing hardware costs</t>
+  </si>
+  <si>
+    <t>To create user interfaces</t>
+  </si>
+  <si>
+    <t>Ensuring the product is ready for delivery</t>
+  </si>
+  <si>
+    <t>A testing technique</t>
+  </si>
+  <si>
+    <t>To run acceptance tests</t>
+  </si>
+  <si>
+    <t>External perspective</t>
+  </si>
+  <si>
+    <t>They are always incomplete</t>
+  </si>
+  <si>
+    <t>After modules are combined</t>
+  </si>
+  <si>
+    <t>That objects automatically save state</t>
+  </si>
+  <si>
+    <t>Informal review</t>
+  </si>
+  <si>
+    <t>Execution flow of objects or actors</t>
+  </si>
+  <si>
+    <t>Requirements specification</t>
+  </si>
+  <si>
+    <t>They exclude stakeholders</t>
+  </si>
+  <si>
+    <t>Testing strategy design</t>
+  </si>
+  <si>
+    <t>They focus on user interface rather than logic</t>
+  </si>
+  <si>
+    <t>Reduced performance</t>
+  </si>
+  <si>
+    <t>The defect impacts real users and may require large-scale fixes</t>
+  </si>
+  <si>
+    <t>Python code cannot be modeled visually</t>
+  </si>
+  <si>
+    <t>Creating user stories</t>
+  </si>
+  <si>
+    <t>Improving GUI design</t>
   </si>
 </sst>
 </file>
@@ -69,21 +380,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Aptos Display"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -91,7 +402,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -99,7 +410,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -107,35 +418,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -143,7 +454,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -151,14 +462,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -166,14 +477,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -181,7 +492,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -189,14 +500,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -542,52 +853,64 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="הדגשה1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="הדגשה2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="הדגשה3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="הדגשה4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="הדגשה5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="הדגשה6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="הערה" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="חישוב" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="טוב" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="טקסט אזהרה" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="טקסט הסברי" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="כותרת" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="כותרת 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="כותרת 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="כותרת 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="כותרת 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="ניטראלי" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="סה&quot;כ" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="פלט" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="קלט" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="רע" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="תא מסומן" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="תא מקושר" xfId="12" builtinId="24" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -603,7 +926,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -919,13 +1242,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F77A68B-DA47-460E-85C5-67EB06CA9EE9}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,30 +1276,628 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>